<commit_message>
plotting ITS2 and 16S, adonis, updating class
</commit_message>
<xml_diff>
--- a/ITS2_Summer_symportal2020/20201214_matsuda_MCL/post_med_seqs/133_20201216_DBV_20201216T011417.seqs.absolute.meta_only.xlsx
+++ b/ITS2_Summer_symportal2020/20201214_matsuda_MCL/post_med_seqs/133_20201216_DBV_20201216T011417.seqs.absolute.meta_only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayle/Desktop/Microbial landscape/ITS2_Summer_symportal2020/Microbial_landscape_MCL/20201214_matsuda_MCL/post_med_seqs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaylematsuda/Desktop/Projects/Mcapitata_microbial_landscape/ITS2_Summer_symportal2020/20201214_matsuda_MCL/post_med_seqs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ACAD1B-A37B-004D-98AB-344978F7E312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF08F7D6-BCC5-804C-A05F-241F18F4E8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="840" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3020" yWindow="1300" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="133_20201216_DBV_20201216T01141" sheetId="1" r:id="rId1"/>
@@ -1778,9 +1778,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1840,7 +1839,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2128,7 +2127,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2139,7 +2138,7 @@
   <dimension ref="A1:AG385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2170,7 +2169,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">

</xml_diff>